<commit_message>
update điểm của bảo duy
</commit_message>
<xml_diff>
--- a/Lop6/2021 - 2022/BTVN/Diem.xlsx
+++ b/Lop6/2021 - 2022/BTVN/Diem.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Điểm</t>
   </si>
@@ -253,6 +253,45 @@
   </si>
   <si>
     <t>BÀI 7. LŨY THỪA VỚI SỐ MŨ TỰ NHIÊN</t>
+  </si>
+  <si>
+    <r>
+      <t>Duy làm bài tốt, con chú ý thêm các vấn đề sau:
+- Con cần làm thêm</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bài 7.
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Các bài toán tìm x cầm có kết luận ở cuối bài.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -639,7 +678,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,12 +712,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -711,13 +752,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>7.5</v>
+      </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">

</xml_diff>